<commit_message>
Update case files in ams_benchmark, renaming model Region to Zone
</commit_message>
<xml_diff>
--- a/demo/ams_benchmark/opf/cases/ieee14_uced.xlsx
+++ b/demo/ams_benchmark/opf/cases/ieee14_uced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/ams/icebar/CaseStudy/opf/cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBE0820-1D01-814B-8325-1212BEBB10A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9774DCD-763B-2646-B84B-D62DC2047955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Shunt" sheetId="6" r:id="rId7"/>
     <sheet name="Area" sheetId="7" r:id="rId8"/>
     <sheet name="GCost" sheetId="8" r:id="rId9"/>
-    <sheet name="Region" sheetId="10" r:id="rId10"/>
+    <sheet name="Zone" sheetId="10" r:id="rId10"/>
     <sheet name="EDTSlot" sheetId="13" r:id="rId11"/>
     <sheet name="UCTSlot" sheetId="14" r:id="rId12"/>
     <sheet name="SFR" sheetId="16" r:id="rId13"/>
@@ -1797,7 +1797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -4148,8 +4148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:V2"/>
+    <sheetView zoomScale="105" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4284,10 +4284,10 @@
         <v>999</v>
       </c>
       <c r="U2" s="1">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="V2" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -4349,10 +4349,10 @@
         <v>999</v>
       </c>
       <c r="U3" s="1">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="V3" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -4414,10 +4414,10 @@
         <v>999</v>
       </c>
       <c r="U4" s="1">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="V4" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -4479,10 +4479,10 @@
         <v>999</v>
       </c>
       <c r="U5" s="1">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="V5" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4498,8 +4498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4640,10 +4640,10 @@
         <v>1</v>
       </c>
       <c r="V2" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W2" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">

</xml_diff>